<commit_message>
fixed attribute names and labels
</commit_message>
<xml_diff>
--- a/emx/portal-demographics/rd3_portal_demographics.xlsx
+++ b/emx/portal-demographics/rd3_portal_demographics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcruvolo/GitHub/molgenis-solve-rd/emx/portal-demographics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57ACA93-AE74-4D48-B68A-3EC56E2BA514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7372B0-70D2-9D4D-9048-9C54F73461B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32000" yWindow="-2880" windowWidth="25440" windowHeight="14840" activeTab="2" xr2:uid="{3259F299-4885-CF44-B001-3E241E2377BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -107,16 +107,28 @@
     <t>sex</t>
   </si>
   <si>
-    <t>observed sex</t>
-  </si>
-  <si>
-    <t>calculated ethnicity</t>
-  </si>
-  <si>
     <t>auto_id</t>
   </si>
   <si>
     <t>auto generated molgenis ID</t>
+  </si>
+  <si>
+    <t>Observed Sex</t>
+  </si>
+  <si>
+    <t>experimentID</t>
+  </si>
+  <si>
+    <t>ExperimentID</t>
+  </si>
+  <si>
+    <t>experiment ID</t>
+  </si>
+  <si>
+    <t>Calculated Ancestry</t>
+  </si>
+  <si>
+    <t>Ancestry that was derived</t>
   </si>
 </sst>
 </file>
@@ -561,13 +573,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD4FE2A-054B-2E47-9E25-0A1F62DD96E6}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -629,13 +647,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -650,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -658,13 +676,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -687,13 +705,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -702,15 +720,44 @@
         <v>20</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>